<commit_message>
grouped directive on multiple columns.
Grouped example now shows how to used with multiple columns
</commit_message>
<xml_diff>
--- a/examples/Grouped example.xlsx
+++ b/examples/Grouped example.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Users\enebo\calculus\gridster-tooling\dev-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4A0573-4720-482B-A739-6D70391B2905}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8B81BAC-711B-47AE-8378-381DE48AF011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="317" yWindow="3634" windowWidth="12077" windowHeight="11306" xr2:uid="{ECDAFFB1-ED7C-46CD-9E0E-9AE8FDDB1639}"/>
   </bookViews>
   <sheets>
-    <sheet name="Deposits" sheetId="1" r:id="rId1"/>
+    <sheet name="Names" sheetId="2" r:id="rId1"/>
+    <sheet name="Deposits" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -27,63 +39,98 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>mark</author>
+    <author>tc={C4889086-F857-4160-BCCE-B2C531C8A5FD}</author>
+    <author>tc={DC0BA95E-7B20-4B79-ABC4-7B8366C2E8BE}</author>
+    <author>tc={D23255C3-B2C1-40C1-A2F7-4A9AF1B28DCD}</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{482886CD-C2F1-415F-B420-B53B95573B2A}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C4889086-F857-4160-BCCE-B2C531C8A5FD}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mark:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-pebblestream:grouped</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    pebblestream:grouped</t>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{F2688D43-A105-44DD-8D15-A92B0B5980F3}">
+    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{DC0BA95E-7B20-4B79-ABC4-7B8366C2E8BE}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>mark:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This will make the runtime throw an exception</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    pebblestream:grouped</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="2" shapeId="0" xr:uid="{D23255C3-B2C1-40C1-A2F7-4A9AF1B28DCD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This will make the runtime throw an exception</t>
       </text>
     </comment>
   </commentList>
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={AE62C24E-9FD4-46C3-A03A-A02713FC639D}</author>
+    <author>tc={B7431CA3-3C28-4E7D-BD0F-23FC206FCB54}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AE62C24E-9FD4-46C3-A03A-A02713FC639D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    pebblestream:grouped</t>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="1" shapeId="0" xr:uid="{B7431CA3-3C28-4E7D-BD0F-23FC206FCB54}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This will make the runtime throw an exception
+**ERROR**
+the values in 'Deposits' row 7 columns A appeared as a previous group, so this sheet is not grouped correctly
+**ERROR END**</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Bill</t>
+  </si>
+  <si>
+    <t>Gates</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
   <si>
     <t>Account ID</t>
   </si>
@@ -107,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,26 +162,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE5E7E8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFACAFB7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCADE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,8 +201,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,6 +222,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Abdulbosit Abdurakhmonov" id="{5C0BF0B9-ABF7-4AED-970E-7EBFAF7F1BDB}" userId="1e51334d42f479e5" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -463,88 +525,190 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2024-11-18T10:12:56.79" personId="{5C0BF0B9-ABF7-4AED-970E-7EBFAF7F1BDB}" id="{C4889086-F857-4160-BCCE-B2C531C8A5FD}">
+    <text>pebblestream:grouped</text>
+  </threadedComment>
+  <threadedComment ref="B1" dT="2024-11-18T10:12:56.79" personId="{5C0BF0B9-ABF7-4AED-970E-7EBFAF7F1BDB}" id="{DC0BA95E-7B20-4B79-ABC4-7B8366C2E8BE}">
+    <text>pebblestream:grouped</text>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2024-11-18T10:12:56.79" personId="{5C0BF0B9-ABF7-4AED-970E-7EBFAF7F1BDB}" id="{D23255C3-B2C1-40C1-A2F7-4A9AF1B28DCD}">
+    <text>This will make the runtime throw an exception</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2024-11-18T10:12:56.79" personId="{5C0BF0B9-ABF7-4AED-970E-7EBFAF7F1BDB}" id="{AE62C24E-9FD4-46C3-A03A-A02713FC639D}">
+    <text>pebblestream:grouped</text>
+  </threadedComment>
+  <threadedComment ref="A7" dT="2024-11-18T10:12:56.79" personId="{5C0BF0B9-ABF7-4AED-970E-7EBFAF7F1BDB}" id="{B7431CA3-3C28-4E7D-BD0F-23FC206FCB54}">
+    <text>This will make the runtime throw an exception
+**ERROR**
+the values in 'Deposits' row 7 columns A appeared as a previous group, so this sheet is not grouped correctly
+**ERROR END**</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126FE4F0-C428-4ACF-B845-44CBE6E4A0B2}">
+  <sheetPr>
+    <tabColor rgb="FFACAFB7"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FE8669-A349-461C-BA59-A6D108FDFD3C}">
+  <sheetPr>
+    <tabColor rgb="FFFFCADE"/>
+  </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col min="1" max="1" width="10.53515625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:2">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
+      <c r="B7" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1">
         <v>88</v>
       </c>
     </row>

</xml_diff>